<commit_message>
Use '|' symbol for lane divider
</commit_message>
<xml_diff>
--- a/Scrum Teams.xlsx
+++ b/Scrum Teams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NikAntonelli\Planview\Development\Groundhog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA517E0D-7F60-4D2E-9A44-046A876CFFD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0436785B-CA10-4784-9B41-B889B66747FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{29CD428F-0A07-48A0-8573-8048C934683D}"/>
+    <workbookView xWindow="-2430" yWindow="-21495" windowWidth="29745" windowHeight="17940" activeTab="1" xr2:uid="{29CD428F-0A07-48A0-8573-8048C934683D}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -121,9 +121,6 @@
     <t>Lane</t>
   </si>
   <si>
-    <t>Review</t>
-  </si>
-  <si>
     <t>Analysis</t>
   </si>
   <si>
@@ -131,6 +128,9 @@
   </si>
   <si>
     <t>My Scheduled Story</t>
+  </si>
+  <si>
+    <t>Implementation per ART/VS|Art 1|In Progress</t>
   </si>
 </sst>
 </file>
@@ -539,7 +539,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E2">
         <v>14</v>
@@ -557,7 +557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8163DD46-63A6-4C19-A83F-CE88989C762C}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -657,7 +657,7 @@
         <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -677,7 +677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{525ADE1B-52CA-4A24-AFEE-91E8EE2AC7BD}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -721,10 +721,10 @@
         <v>26</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H2" t="s">
         <v>22</v>

</xml_diff>